<commit_message>
Add variables 'Num_Books' and 'Fav_Genre'
Created variables for the number of books read in last year ('num_books') and favorite genre of book ('fav_genre')
</commit_message>
<xml_diff>
--- a/data/raw_data/exampledata.xlsx
+++ b/data/raw_data/exampledata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F6676E-8A84-4027-81F4-2285066F9254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A823644E-C7C1-4493-AE5F-CC26A7C51F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="420" windowWidth="44640" windowHeight="21645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
   <si>
     <t>Height</t>
   </si>
@@ -57,6 +57,24 @@
   </si>
   <si>
     <t>height in centimeters</t>
+  </si>
+  <si>
+    <t>Num_Books</t>
+  </si>
+  <si>
+    <t>Fav_Genre</t>
+  </si>
+  <si>
+    <t>Sci-Fi</t>
+  </si>
+  <si>
+    <t>Horror</t>
+  </si>
+  <si>
+    <t>Romance</t>
+  </si>
+  <si>
+    <t>Dark Comedy</t>
   </si>
 </sst>
 </file>
@@ -383,15 +401,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -401,8 +419,14 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>180</v>
       </c>
@@ -412,8 +436,14 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>175</v>
       </c>
@@ -423,8 +453,14 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -434,8 +470,14 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>178</v>
       </c>
@@ -445,8 +487,14 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>192</v>
       </c>
@@ -456,8 +504,14 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -467,8 +521,14 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>156</v>
       </c>
@@ -478,8 +538,14 @@
       <c r="C8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>166</v>
       </c>
@@ -489,8 +555,14 @@
       <c r="C9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>155</v>
       </c>
@@ -500,8 +572,14 @@
       <c r="C10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>145</v>
       </c>
@@ -511,16 +589,28 @@
       <c r="C11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>165</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>133</v>
       </c>
@@ -530,8 +620,14 @@
       <c r="C13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>166</v>
       </c>
@@ -541,8 +637,14 @@
       <c r="C14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>154</v>
       </c>
@@ -552,9 +654,16 @@
       <c r="C15" t="s">
         <v>4</v>
       </c>
+      <c r="D15">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -566,13 +675,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -580,7 +689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -588,7 +697,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -596,7 +705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>

</xml_diff>